<commit_message>
Städning 13 april 2021
</commit_message>
<xml_diff>
--- a/Bibsam_tidskriftslistor/scifree_data_cambridge.xlsx
+++ b/Bibsam_tidskriftslistor/scifree_data_cambridge.xlsx
@@ -4437,28 +4437,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -4736,7 +4715,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G371"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>